<commit_message>
Updating XLSX with additional sheets.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/test_1header.xlsx
+++ b/src/test/resources/xls/test_1header.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkryzwicki\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\sentinel\src\test\resources\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A5C7D7-E088-45C6-9D42-1DE09413DD6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0800CC-35F6-497C-BD56-A75073AE3A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33435" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Random" sheetId="1" r:id="rId1"/>
+    <sheet name="NFL" sheetId="2" r:id="rId2"/>
+    <sheet name="Games" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Title</t>
   </si>
@@ -52,6 +54,57 @@
   </si>
   <si>
     <t>Criss</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Buffalo</t>
+  </si>
+  <si>
+    <t>Bills</t>
+  </si>
+  <si>
+    <t>Miami</t>
+  </si>
+  <si>
+    <t>Dolphins</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Broncos</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Fallout 76</t>
+  </si>
+  <si>
+    <t>Bethesda</t>
+  </si>
+  <si>
+    <t>Half-Life</t>
+  </si>
+  <si>
+    <t>Valve</t>
+  </si>
+  <si>
+    <t>Doom</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Duke Nukem</t>
+  </si>
+  <si>
+    <t>3D Realms</t>
+  </si>
+  <si>
+    <t>Team Name</t>
   </si>
 </sst>
 </file>
@@ -371,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,4 +469,113 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC997070-7D3F-43BF-B6D5-BC36D9019D9B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3485622-E15C-4BC5-B435-A72392A21364}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>